<commit_message>
added printable to api
</commit_message>
<xml_diff>
--- a/pdf-manager/Disbursement.xlsx
+++ b/pdf-manager/Disbursement.xlsx
@@ -73,7 +73,7 @@
     <t>Peter Buonaiuto</t>
   </si>
   <si>
-    <t xml:space="preserve">201 Greenbelt PKWY </t>
+    <t xml:space="preserve">201 Greenbelt </t>
   </si>
   <si>
     <t xml:space="preserve">My Account </t>
@@ -454,7 +454,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>

</xml_diff>